<commit_message>
Database Table modified in db-tables.xsl and Project synopsis finalized in project-details folder
</commit_message>
<xml_diff>
--- a/project-details/db-tables.xlsx
+++ b/project-details/db-tables.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="131">
   <si>
     <t>id</t>
   </si>
@@ -261,13 +261,154 @@
     <t>credit card transaction</t>
   </si>
   <si>
-    <t>table name : cc</t>
-  </si>
-  <si>
     <t>Helpline-user</t>
   </si>
   <si>
     <t>Bank-Transaction</t>
+  </si>
+  <si>
+    <t>nominee-name</t>
+  </si>
+  <si>
+    <t>nominee-id</t>
+  </si>
+  <si>
+    <t>r-name</t>
+  </si>
+  <si>
+    <t>table name : card-no</t>
+  </si>
+  <si>
+    <t>applies</t>
+  </si>
+  <si>
+    <t>approved</t>
+  </si>
+  <si>
+    <t>deleivered</t>
+  </si>
+  <si>
+    <t>deactivated</t>
+  </si>
+  <si>
+    <t>application-no</t>
+  </si>
+  <si>
+    <t>loan</t>
+  </si>
+  <si>
+    <t>loan-ac-no</t>
+  </si>
+  <si>
+    <t>adhar card-no</t>
+  </si>
+  <si>
+    <t>pan-card-no</t>
+  </si>
+  <si>
+    <t>home-loan</t>
+  </si>
+  <si>
+    <t>land-detail</t>
+  </si>
+  <si>
+    <t>guranteer-name</t>
+  </si>
+  <si>
+    <t>guranteer-ac-no</t>
+  </si>
+  <si>
+    <t>guaranteer-id</t>
+  </si>
+  <si>
+    <t>guaranteer-photo</t>
+  </si>
+  <si>
+    <t>guranteer-signature</t>
+  </si>
+  <si>
+    <t>study-loan</t>
+  </si>
+  <si>
+    <t>bonafite-certificate</t>
+  </si>
+  <si>
+    <t>fee-structure</t>
+  </si>
+  <si>
+    <t>affidevit</t>
+  </si>
+  <si>
+    <t>current address</t>
+  </si>
+  <si>
+    <t>personal-loan</t>
+  </si>
+  <si>
+    <t>purpose</t>
+  </si>
+  <si>
+    <t>application no</t>
+  </si>
+  <si>
+    <t>car-loan</t>
+  </si>
+  <si>
+    <t>agency-detail</t>
+  </si>
+  <si>
+    <t>land-details</t>
+  </si>
+  <si>
+    <t>branches</t>
+  </si>
+  <si>
+    <t>branch-code</t>
+  </si>
+  <si>
+    <t>manager-name</t>
+  </si>
+  <si>
+    <t>loan-type</t>
+  </si>
+  <si>
+    <t>rate</t>
+  </si>
+  <si>
+    <t>study</t>
+  </si>
+  <si>
+    <t>home</t>
+  </si>
+  <si>
+    <t>personal</t>
+  </si>
+  <si>
+    <t>car</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>joining date</t>
+  </si>
+  <si>
+    <t>adhar-no</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FD </t>
+  </si>
+  <si>
+    <t>adhar card</t>
+  </si>
+  <si>
+    <t>pan-card (jpg)</t>
+  </si>
+  <si>
+    <t>adhar-card (jpg)</t>
+  </si>
+  <si>
+    <t>year</t>
   </si>
 </sst>
 </file>
@@ -323,12 +464,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -623,35 +767,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BA35"/>
+  <dimension ref="A1:BD63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="C69" sqref="C69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.7109375" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.28515625" customWidth="1"/>
     <col min="6" max="6" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="18" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10" customWidth="1"/>
-    <col min="19" max="19" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="19" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="11.42578125" bestFit="1" customWidth="1"/>
@@ -681,14 +824,17 @@
     <col min="51" max="51" width="4" bestFit="1" customWidth="1"/>
     <col min="52" max="52" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="53" max="53" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53">
+    <row r="1" spans="1:56">
       <c r="A1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:53">
+    <row r="2" spans="1:56">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -848,13 +994,22 @@
       <c r="BA2" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="4" spans="1:53">
+      <c r="BB2" t="s">
+        <v>83</v>
+      </c>
+      <c r="BC2" t="s">
+        <v>84</v>
+      </c>
+      <c r="BD2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:56">
       <c r="A4" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="5" spans="1:53">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="5" spans="1:56">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -877,17 +1032,17 @@
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:53">
+    <row r="7" spans="1:56">
       <c r="A7" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:53">
+    <row r="8" spans="1:56">
       <c r="A8" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="1:53">
+    <row r="9" spans="1:56">
       <c r="A9" s="1" t="s">
         <v>0</v>
       </c>
@@ -907,17 +1062,17 @@
         <v>58</v>
       </c>
     </row>
-    <row r="10" spans="1:53">
+    <row r="10" spans="1:56">
       <c r="D10" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="12" spans="1:53">
+    <row r="12" spans="1:56">
       <c r="A12" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="13" spans="1:53">
+    <row r="13" spans="1:56">
       <c r="A13" s="1" t="s">
         <v>0</v>
       </c>
@@ -1033,12 +1188,20 @@
         <v>62</v>
       </c>
     </row>
-    <row r="15" spans="1:53">
+    <row r="14" spans="1:56">
+      <c r="AI14" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:56">
       <c r="A15" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="16" spans="1:53">
+      <c r="AI15" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:56">
       <c r="A16" s="1" t="s">
         <v>0</v>
       </c>
@@ -1103,7 +1266,7 @@
     </row>
     <row r="21" spans="1:34">
       <c r="A21" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="22" spans="1:34">
@@ -1260,15 +1423,18 @@
         <v>72</v>
       </c>
       <c r="G28" t="s">
+        <v>85</v>
+      </c>
+      <c r="H28" t="s">
         <v>73</v>
       </c>
-      <c r="H28" s="2" t="s">
+      <c r="I28" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="I28" s="4" t="s">
+      <c r="J28" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="J28" t="s">
+      <c r="K28" t="s">
         <v>62</v>
       </c>
     </row>
@@ -1308,20 +1474,533 @@
       <c r="J31" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="33" spans="1:1">
+      <c r="K31" t="s">
+        <v>62</v>
+      </c>
+      <c r="L31" t="s">
+        <v>91</v>
+      </c>
+      <c r="M31" t="s">
+        <v>31</v>
+      </c>
+      <c r="N31" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="32" spans="1:34">
+      <c r="K32" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="33" spans="1:24">
       <c r="A33" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="34" spans="1:1">
+      <c r="K33" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="34" spans="1:24">
       <c r="A34" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1">
+        <v>86</v>
+      </c>
+      <c r="K34" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="35" spans="1:24">
       <c r="A35" s="1" t="s">
         <v>0</v>
+      </c>
+      <c r="B35" t="s">
+        <v>54</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F35" t="s">
+        <v>72</v>
+      </c>
+      <c r="K35" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="37" spans="1:24">
+      <c r="A37" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="38" spans="1:24">
+      <c r="A38" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B38" t="s">
+        <v>2</v>
+      </c>
+      <c r="C38" t="s">
+        <v>33</v>
+      </c>
+      <c r="D38" t="s">
+        <v>34</v>
+      </c>
+      <c r="E38" t="s">
+        <v>93</v>
+      </c>
+      <c r="F38" t="s">
+        <v>19</v>
+      </c>
+      <c r="G38" t="s">
+        <v>20</v>
+      </c>
+      <c r="H38" t="s">
+        <v>3</v>
+      </c>
+      <c r="I38" t="s">
+        <v>94</v>
+      </c>
+      <c r="J38" t="s">
+        <v>95</v>
+      </c>
+      <c r="K38" t="s">
+        <v>97</v>
+      </c>
+      <c r="L38" t="s">
+        <v>31</v>
+      </c>
+      <c r="M38" t="s">
+        <v>32</v>
+      </c>
+      <c r="N38" t="s">
+        <v>98</v>
+      </c>
+      <c r="O38" t="s">
+        <v>99</v>
+      </c>
+      <c r="P38" t="s">
+        <v>100</v>
+      </c>
+      <c r="Q38" t="s">
+        <v>101</v>
+      </c>
+      <c r="R38" t="s">
+        <v>102</v>
+      </c>
+      <c r="S38" t="s">
+        <v>107</v>
+      </c>
+      <c r="T38" t="s">
+        <v>110</v>
+      </c>
+      <c r="U38" t="s">
+        <v>57</v>
+      </c>
+      <c r="V38" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="40" spans="1:24">
+      <c r="A40" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="41" spans="1:24">
+      <c r="A41" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B41" t="s">
+        <v>2</v>
+      </c>
+      <c r="C41" t="s">
+        <v>33</v>
+      </c>
+      <c r="D41" t="s">
+        <v>34</v>
+      </c>
+      <c r="E41" t="s">
+        <v>93</v>
+      </c>
+      <c r="F41" t="s">
+        <v>19</v>
+      </c>
+      <c r="G41" t="s">
+        <v>20</v>
+      </c>
+      <c r="H41" t="s">
+        <v>3</v>
+      </c>
+      <c r="I41" t="s">
+        <v>94</v>
+      </c>
+      <c r="J41" t="s">
+        <v>95</v>
+      </c>
+      <c r="K41" t="s">
+        <v>104</v>
+      </c>
+      <c r="L41" t="s">
+        <v>31</v>
+      </c>
+      <c r="M41" t="s">
+        <v>32</v>
+      </c>
+      <c r="N41" t="s">
+        <v>98</v>
+      </c>
+      <c r="O41" t="s">
+        <v>99</v>
+      </c>
+      <c r="P41" t="s">
+        <v>100</v>
+      </c>
+      <c r="Q41" t="s">
+        <v>101</v>
+      </c>
+      <c r="R41" t="s">
+        <v>102</v>
+      </c>
+      <c r="S41" t="s">
+        <v>105</v>
+      </c>
+      <c r="T41" t="s">
+        <v>106</v>
+      </c>
+      <c r="U41" t="s">
+        <v>107</v>
+      </c>
+      <c r="V41" t="s">
+        <v>110</v>
+      </c>
+      <c r="W41" t="s">
+        <v>57</v>
+      </c>
+      <c r="X41" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="43" spans="1:24">
+      <c r="A43" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="44" spans="1:24">
+      <c r="A44" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B44" t="s">
+        <v>2</v>
+      </c>
+      <c r="C44" t="s">
+        <v>33</v>
+      </c>
+      <c r="D44" t="s">
+        <v>34</v>
+      </c>
+      <c r="E44" t="s">
+        <v>93</v>
+      </c>
+      <c r="F44" t="s">
+        <v>19</v>
+      </c>
+      <c r="G44" t="s">
+        <v>20</v>
+      </c>
+      <c r="H44" t="s">
+        <v>3</v>
+      </c>
+      <c r="I44" t="s">
+        <v>94</v>
+      </c>
+      <c r="J44" t="s">
+        <v>95</v>
+      </c>
+      <c r="K44" t="s">
+        <v>109</v>
+      </c>
+      <c r="L44" t="s">
+        <v>31</v>
+      </c>
+      <c r="M44" t="s">
+        <v>32</v>
+      </c>
+      <c r="N44" t="s">
+        <v>98</v>
+      </c>
+      <c r="O44" t="s">
+        <v>99</v>
+      </c>
+      <c r="P44" t="s">
+        <v>100</v>
+      </c>
+      <c r="Q44" t="s">
+        <v>101</v>
+      </c>
+      <c r="R44" t="s">
+        <v>102</v>
+      </c>
+      <c r="S44" t="s">
+        <v>107</v>
+      </c>
+      <c r="T44" t="s">
+        <v>110</v>
+      </c>
+      <c r="U44" t="s">
+        <v>57</v>
+      </c>
+      <c r="V44" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="46" spans="1:24">
+      <c r="A46" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="47" spans="1:24">
+      <c r="A47" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B47" t="s">
+        <v>2</v>
+      </c>
+      <c r="C47" t="s">
+        <v>33</v>
+      </c>
+      <c r="D47" t="s">
+        <v>34</v>
+      </c>
+      <c r="E47" t="s">
+        <v>93</v>
+      </c>
+      <c r="F47" t="s">
+        <v>19</v>
+      </c>
+      <c r="G47" t="s">
+        <v>20</v>
+      </c>
+      <c r="H47" t="s">
+        <v>3</v>
+      </c>
+      <c r="I47" t="s">
+        <v>94</v>
+      </c>
+      <c r="J47" t="s">
+        <v>95</v>
+      </c>
+      <c r="K47" t="s">
+        <v>112</v>
+      </c>
+      <c r="L47" t="s">
+        <v>31</v>
+      </c>
+      <c r="M47" t="s">
+        <v>32</v>
+      </c>
+      <c r="N47" t="s">
+        <v>98</v>
+      </c>
+      <c r="O47" t="s">
+        <v>99</v>
+      </c>
+      <c r="P47" t="s">
+        <v>100</v>
+      </c>
+      <c r="Q47" t="s">
+        <v>101</v>
+      </c>
+      <c r="R47" t="s">
+        <v>102</v>
+      </c>
+      <c r="S47" t="s">
+        <v>107</v>
+      </c>
+      <c r="T47" t="s">
+        <v>110</v>
+      </c>
+      <c r="U47" t="s">
+        <v>113</v>
+      </c>
+      <c r="V47" t="s">
+        <v>57</v>
+      </c>
+      <c r="W47" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="49" spans="1:19">
+      <c r="A49" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="50" spans="1:19">
+      <c r="A50" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B50" t="s">
+        <v>1</v>
+      </c>
+      <c r="C50" t="s">
+        <v>115</v>
+      </c>
+      <c r="D50" t="s">
+        <v>25</v>
+      </c>
+      <c r="E50" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="52" spans="1:19">
+      <c r="A52" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="53" spans="1:19">
+      <c r="A53" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B53" t="s">
+        <v>117</v>
+      </c>
+      <c r="C53" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="54" spans="1:19">
+      <c r="B54" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="55" spans="1:19">
+      <c r="B55" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="56" spans="1:19">
+      <c r="B56" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="57" spans="1:19">
+      <c r="B57" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="59" spans="1:19">
+      <c r="A59" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="60" spans="1:19">
+      <c r="A60" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B60" t="s">
+        <v>1</v>
+      </c>
+      <c r="C60" t="s">
+        <v>116</v>
+      </c>
+      <c r="D60" t="s">
+        <v>19</v>
+      </c>
+      <c r="E60" t="s">
+        <v>20</v>
+      </c>
+      <c r="F60" t="s">
+        <v>124</v>
+      </c>
+      <c r="G60" t="s">
+        <v>3</v>
+      </c>
+      <c r="H60" t="s">
+        <v>25</v>
+      </c>
+      <c r="I60" t="s">
+        <v>31</v>
+      </c>
+      <c r="J60" t="s">
+        <v>32</v>
+      </c>
+      <c r="K60" t="s">
+        <v>125</v>
+      </c>
+      <c r="L60" t="s">
+        <v>18</v>
+      </c>
+      <c r="M60" t="s">
+        <v>129</v>
+      </c>
+      <c r="N60" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="62" spans="1:19">
+      <c r="A62" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="63" spans="1:19">
+      <c r="A63" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B63" t="s">
+        <v>1</v>
+      </c>
+      <c r="C63" t="s">
+        <v>91</v>
+      </c>
+      <c r="D63" t="s">
+        <v>2</v>
+      </c>
+      <c r="E63" t="s">
+        <v>34</v>
+      </c>
+      <c r="F63" t="s">
+        <v>33</v>
+      </c>
+      <c r="G63" t="s">
+        <v>3</v>
+      </c>
+      <c r="H63" t="s">
+        <v>19</v>
+      </c>
+      <c r="I63" t="s">
+        <v>20</v>
+      </c>
+      <c r="J63" t="s">
+        <v>31</v>
+      </c>
+      <c r="K63" t="s">
+        <v>32</v>
+      </c>
+      <c r="L63" t="s">
+        <v>125</v>
+      </c>
+      <c r="M63" t="s">
+        <v>18</v>
+      </c>
+      <c r="N63" t="s">
+        <v>128</v>
+      </c>
+      <c r="O63" t="s">
+        <v>127</v>
+      </c>
+      <c r="P63" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q63" t="s">
+        <v>57</v>
+      </c>
+      <c r="R63" t="s">
+        <v>62</v>
+      </c>
+      <c r="S63" t="s">
+        <v>130</v>
       </c>
     </row>
   </sheetData>

</xml_diff>